<commit_message>
change in brand entry
</commit_message>
<xml_diff>
--- a/public/excel/BrandDetailsNew.xlsx
+++ b/public/excel/BrandDetailsNew.xlsx
@@ -62,7 +62,7 @@
     <t>Samsung A-21</t>
   </si>
   <si>
-    <t>Airtel</t>
+    <t>Idea</t>
   </si>
   <si>
     <t>Admin Admin</t>
@@ -501,10 +501,10 @@
         <v>12</v>
       </c>
       <c r="D2" s="1">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2">
-        <v>7888777888</v>
+        <v>7405383061</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -536,10 +536,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="1">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="E3" s="2">
-        <v>7888777888</v>
+        <v>7405383061</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>19</v>
@@ -571,10 +571,10 @@
         <v>21</v>
       </c>
       <c r="D4" s="1">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="E4" s="2">
-        <v>7888777888</v>
+        <v>7405383061</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>19</v>
@@ -606,10 +606,10 @@
         <v>23</v>
       </c>
       <c r="D5" s="1">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="E5" s="2">
-        <v>7888777888</v>
+        <v>7405383061</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>19</v>
@@ -641,10 +641,10 @@
         <v>25</v>
       </c>
       <c r="D6" s="1">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="E6" s="2">
-        <v>7888777888</v>
+        <v>7405383061</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>13</v>

</xml_diff>